<commit_message>
Ordenamiento de urls en drive Basculas
</commit_message>
<xml_diff>
--- a/PULIR/Termometros/pulido.xlsx
+++ b/PULIR/Termometros/pulido.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="241">
   <si>
     <t>CENTRO DE SALUD SANTA LUCIA</t>
   </si>
@@ -639,6 +639,18 @@
     <t>GSP-6</t>
   </si>
   <si>
+    <t>T13081124133</t>
+  </si>
+  <si>
+    <t>IN 133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M7 </t>
+  </si>
+  <si>
+    <t>PROCEDIMIENTOS MENORES</t>
+  </si>
+  <si>
     <t>V010711241596</t>
   </si>
   <si>
@@ -1003,7 +1015,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="120">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1234,6 +1246,21 @@
     </xf>
     <xf borderId="10" fillId="0" fontId="8" numFmtId="172" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -12457,7 +12484,7 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="12" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -24115,24 +24142,356 @@
       </c>
     </row>
     <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1">
+      <c r="A229" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B229" s="2"/>
+      <c r="C229" s="2"/>
+      <c r="D229" s="2"/>
+      <c r="E229" s="2"/>
+      <c r="F229" s="2"/>
+      <c r="G229" s="2"/>
+      <c r="H229" s="2"/>
+      <c r="I229" s="2"/>
+      <c r="J229" s="2"/>
+      <c r="K229" s="3"/>
+    </row>
+    <row r="230" ht="15.75" customHeight="1">
+      <c r="A230" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B230" s="3"/>
+      <c r="C230" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D230" s="2"/>
+      <c r="E230" s="2"/>
+      <c r="F230" s="2"/>
+      <c r="G230" s="2"/>
+      <c r="H230" s="2"/>
+      <c r="I230" s="2"/>
+      <c r="J230" s="2"/>
+      <c r="K230" s="3"/>
+    </row>
+    <row r="231" ht="15.75" customHeight="1">
+      <c r="A231" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B231" s="3"/>
+      <c r="C231" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D231" s="2"/>
+      <c r="E231" s="2"/>
+      <c r="F231" s="2"/>
+      <c r="G231" s="2"/>
+      <c r="H231" s="2"/>
+      <c r="I231" s="2"/>
+      <c r="J231" s="2"/>
+      <c r="K231" s="3"/>
+    </row>
+    <row r="232" ht="15.75" customHeight="1">
+      <c r="A232" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B232" s="3"/>
+      <c r="C232" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D232" s="2"/>
+      <c r="E232" s="2"/>
+      <c r="F232" s="2"/>
+      <c r="G232" s="2"/>
+      <c r="H232" s="2"/>
+      <c r="I232" s="2"/>
+      <c r="J232" s="2"/>
+      <c r="K232" s="3"/>
+    </row>
+    <row r="233" ht="15.75" customHeight="1">
+      <c r="A233" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B233" s="3"/>
+      <c r="C233" s="5">
+        <v>7289584.0</v>
+      </c>
+      <c r="D233" s="2"/>
+      <c r="E233" s="2"/>
+      <c r="F233" s="2"/>
+      <c r="G233" s="2"/>
+      <c r="H233" s="2"/>
+      <c r="I233" s="2"/>
+      <c r="J233" s="2"/>
+      <c r="K233" s="3"/>
+    </row>
+    <row r="234" ht="15.75" customHeight="1">
+      <c r="A234" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B234" s="2"/>
+      <c r="C234" s="2"/>
+      <c r="D234" s="2"/>
+      <c r="E234" s="3"/>
+      <c r="F234" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G234" s="3"/>
+      <c r="H234" s="103" t="s">
+        <v>207</v>
+      </c>
+      <c r="I234" s="2"/>
+      <c r="J234" s="2"/>
+      <c r="K234" s="3"/>
+    </row>
+    <row r="235" ht="15.75" customHeight="1">
+      <c r="A235" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B235" s="3"/>
+      <c r="C235" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D235" s="2"/>
+      <c r="E235" s="3"/>
+      <c r="F235" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G235" s="3"/>
+      <c r="H235" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="I235" s="2"/>
+      <c r="J235" s="2"/>
+      <c r="K235" s="3"/>
+    </row>
+    <row r="236" ht="15.75" customHeight="1">
+      <c r="A236" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B236" s="14"/>
+      <c r="C236" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="D236" s="2"/>
+      <c r="E236" s="3"/>
+      <c r="F236" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G236" s="3"/>
+      <c r="H236" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="I236" s="2"/>
+      <c r="J236" s="2"/>
+      <c r="K236" s="3"/>
+    </row>
+    <row r="237" ht="15.75" customHeight="1">
+      <c r="A237" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B237" s="3"/>
+      <c r="C237" s="41">
+        <v>133.0</v>
+      </c>
+      <c r="D237" s="2"/>
+      <c r="E237" s="3"/>
+      <c r="F237" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G237" s="3"/>
+      <c r="H237" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="I237" s="2"/>
+      <c r="J237" s="2"/>
+      <c r="K237" s="3"/>
+    </row>
+    <row r="238" ht="15.75" customHeight="1">
+      <c r="A238" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="B238" s="25">
+        <v>26.78</v>
+      </c>
+      <c r="C238" s="96">
+        <v>30.58</v>
+      </c>
+      <c r="D238" s="96">
+        <v>32.68</v>
+      </c>
+      <c r="E238" s="96">
+        <v>34.82</v>
+      </c>
+      <c r="F238" s="96">
+        <v>36.46</v>
+      </c>
+      <c r="G238" s="96">
+        <v>38.58</v>
+      </c>
+      <c r="H238" s="96"/>
+      <c r="I238" s="96"/>
+      <c r="J238" s="23"/>
+      <c r="K238" s="23"/>
+    </row>
+    <row r="239" ht="15.75" customHeight="1">
+      <c r="A239" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B239" s="104">
+        <v>26.6</v>
+      </c>
+      <c r="C239" s="105">
+        <v>30.0</v>
+      </c>
+      <c r="D239" s="106">
+        <v>32.1</v>
+      </c>
+      <c r="E239" s="106">
+        <v>34.3</v>
+      </c>
+      <c r="F239" s="106">
+        <v>35.9</v>
+      </c>
+      <c r="G239" s="107">
+        <v>38.0</v>
+      </c>
+      <c r="H239" s="46"/>
+      <c r="I239" s="46"/>
+      <c r="J239" s="40"/>
+      <c r="K239" s="23"/>
+    </row>
+    <row r="240" ht="15.75" customHeight="1">
+      <c r="A240" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B240" s="52">
+        <f t="shared" ref="B240:G240" si="13">B238-B239</f>
+        <v>0.18</v>
+      </c>
+      <c r="C240" s="52">
+        <f t="shared" si="13"/>
+        <v>0.58</v>
+      </c>
+      <c r="D240" s="52">
+        <f t="shared" si="13"/>
+        <v>0.58</v>
+      </c>
+      <c r="E240" s="52">
+        <f t="shared" si="13"/>
+        <v>0.52</v>
+      </c>
+      <c r="F240" s="52">
+        <f t="shared" si="13"/>
+        <v>0.56</v>
+      </c>
+      <c r="G240" s="52">
+        <f t="shared" si="13"/>
+        <v>0.58</v>
+      </c>
+      <c r="H240" s="52"/>
+      <c r="I240" s="52"/>
+      <c r="J240" s="23"/>
+      <c r="K240" s="23"/>
+    </row>
+    <row r="241" ht="15.75" customHeight="1">
+      <c r="A241" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B241" s="102">
+        <f>(B240+C240+D240+E240+F240+D242)/6</f>
+        <v>0.4033333333</v>
+      </c>
+      <c r="C241" s="83"/>
+      <c r="D241" s="50"/>
+      <c r="E241" s="50"/>
+      <c r="F241" s="50"/>
+      <c r="G241" s="50"/>
+      <c r="H241" s="23"/>
+      <c r="I241" s="23"/>
+      <c r="J241" s="23"/>
+      <c r="K241" s="23"/>
+    </row>
+    <row r="242" ht="15.75" customHeight="1">
+      <c r="A242" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B242" s="99">
+        <f>STDEV(B240:G240)
+</f>
+        <v>0.158492902</v>
+      </c>
+      <c r="C242" s="83"/>
+      <c r="D242" s="50"/>
+      <c r="E242" s="50"/>
+      <c r="F242" s="50"/>
+      <c r="G242" s="50"/>
+      <c r="H242" s="23"/>
+      <c r="I242" s="23"/>
+      <c r="J242" s="23"/>
+      <c r="K242" s="23"/>
+    </row>
+    <row r="243" ht="15.75" customHeight="1">
+      <c r="A243" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B243" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C243" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D243" s="35">
+        <f>B242/SQRT(6)</f>
+        <v>0.06470445631</v>
+      </c>
+      <c r="E243" s="23"/>
+      <c r="F243" s="23"/>
+      <c r="G243" s="23"/>
+      <c r="H243" s="23"/>
+      <c r="I243" s="23"/>
+      <c r="J243" s="23"/>
+      <c r="K243" s="23"/>
+    </row>
+    <row r="244" ht="15.75" customHeight="1">
+      <c r="A244" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B244" s="36">
+        <f>SQRT(D243^2 + D244^2 + D245^2)
+</f>
+        <v>0.5627492041</v>
+      </c>
+      <c r="C244" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D244" s="34">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="245" ht="15.75" customHeight="1">
+      <c r="A245" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="B245" s="36">
+        <f>B244*2</f>
+        <v>1.125498408</v>
+      </c>
+      <c r="C245" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D245" s="34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="246" ht="15.75" customHeight="1">
+      <c r="A246" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B246" s="40" t="s">
+        <v>170</v>
+      </c>
+    </row>
     <row r="247" ht="15.75" customHeight="1"/>
     <row r="248" ht="15.75" customHeight="1"/>
     <row r="249" ht="15.75" customHeight="1"/>
@@ -24822,7 +25181,7 @@
     <row r="933" ht="15.75" customHeight="1"/>
     <row r="934" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="288">
+  <mergeCells count="312">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:K2"/>
@@ -24960,6 +25319,34 @@
     <mergeCell ref="A215:E215"/>
     <mergeCell ref="F215:G215"/>
     <mergeCell ref="H215:K215"/>
+    <mergeCell ref="A216:B216"/>
+    <mergeCell ref="C216:E216"/>
+    <mergeCell ref="F216:G216"/>
+    <mergeCell ref="H216:K216"/>
+    <mergeCell ref="C217:E217"/>
+    <mergeCell ref="F217:G217"/>
+    <mergeCell ref="H217:K217"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A218:B218"/>
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="F218:G218"/>
+    <mergeCell ref="H218:K218"/>
+    <mergeCell ref="A229:K229"/>
+    <mergeCell ref="C230:K230"/>
+    <mergeCell ref="A230:B230"/>
+    <mergeCell ref="A231:B231"/>
+    <mergeCell ref="C231:K231"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="C232:K232"/>
+    <mergeCell ref="A233:B233"/>
+    <mergeCell ref="C233:K233"/>
+    <mergeCell ref="A234:E234"/>
+    <mergeCell ref="F234:G234"/>
+    <mergeCell ref="H234:K234"/>
+    <mergeCell ref="A235:B235"/>
+    <mergeCell ref="C235:E235"/>
+    <mergeCell ref="F235:G235"/>
+    <mergeCell ref="H235:K235"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="H27:K27"/>
@@ -24997,18 +25384,14 @@
     <mergeCell ref="C60:K60"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="C61:K61"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A218:B218"/>
-    <mergeCell ref="C218:E218"/>
-    <mergeCell ref="F218:G218"/>
-    <mergeCell ref="H218:K218"/>
-    <mergeCell ref="A216:B216"/>
-    <mergeCell ref="C216:E216"/>
-    <mergeCell ref="F216:G216"/>
-    <mergeCell ref="H216:K216"/>
-    <mergeCell ref="C217:E217"/>
-    <mergeCell ref="F217:G217"/>
-    <mergeCell ref="H217:K217"/>
+    <mergeCell ref="A236:B236"/>
+    <mergeCell ref="C236:E236"/>
+    <mergeCell ref="F236:G236"/>
+    <mergeCell ref="H236:K236"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="C237:E237"/>
+    <mergeCell ref="F237:G237"/>
+    <mergeCell ref="H237:K237"/>
     <mergeCell ref="C85:E85"/>
     <mergeCell ref="F85:G85"/>
     <mergeCell ref="A96:K96"/>
@@ -25224,11 +25607,11 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="103" t="s">
+      <c r="F6" s="108" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -25240,7 +25623,7 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="12" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
@@ -25261,7 +25644,7 @@
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="15" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="17"/>
@@ -25299,19 +25682,19 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="B10" s="104" t="s">
-        <v>211</v>
+        <v>214</v>
+      </c>
+      <c r="B10" s="109" t="s">
+        <v>215</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D10" s="79" t="s">
-        <v>213</v>
-      </c>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
+        <v>217</v>
+      </c>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
@@ -25322,7 +25705,7 @@
       <c r="A11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="106">
+      <c r="B11" s="111">
         <v>5.0</v>
       </c>
       <c r="C11" s="79">
@@ -25331,8 +25714,8 @@
       <c r="D11" s="79">
         <v>50.1</v>
       </c>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
@@ -25349,11 +25732,11 @@
       <c r="C12" s="79">
         <v>24.7</v>
       </c>
-      <c r="D12" s="106">
+      <c r="D12" s="111">
         <v>50.0</v>
       </c>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="110"/>
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
@@ -25362,7 +25745,7 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="28" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B13" s="79">
         <v>4.9</v>
@@ -25383,7 +25766,7 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="66" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B14" s="79">
         <v>4.9</v>
@@ -25391,7 +25774,7 @@
       <c r="C14" s="79">
         <v>24.8</v>
       </c>
-      <c r="D14" s="106">
+      <c r="D14" s="111">
         <v>50.0</v>
       </c>
       <c r="E14" s="37"/>
@@ -25404,7 +25787,7 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="66" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B15" s="79">
         <v>5.1</v>
@@ -25425,7 +25808,7 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="66" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B16" s="79">
         <v>4.8</v>
@@ -25449,13 +25832,13 @@
         <v>28</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
@@ -25470,7 +25853,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
@@ -25487,7 +25870,7 @@
         <v>30</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
@@ -25618,11 +26001,11 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="107" t="s">
+      <c r="F29" s="112" t="s">
         <v>13</v>
       </c>
       <c r="H29" s="87" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -25634,7 +26017,7 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="88" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="3"/>
@@ -25643,7 +26026,7 @@
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="88" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -25654,8 +26037,8 @@
         <v>18</v>
       </c>
       <c r="B31" s="14"/>
-      <c r="C31" s="108" t="s">
-        <v>225</v>
+      <c r="C31" s="113" t="s">
+        <v>229</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="17"/>
@@ -25675,7 +26058,7 @@
         <v>22</v>
       </c>
       <c r="B32" s="14"/>
-      <c r="C32" s="109">
+      <c r="C32" s="114">
         <v>244.0</v>
       </c>
       <c r="D32" s="2"/>
@@ -25693,9 +26076,9 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="B33" s="104">
+        <v>214</v>
+      </c>
+      <c r="B33" s="109">
         <v>100.0</v>
       </c>
       <c r="C33" s="79">
@@ -25704,8 +26087,8 @@
       <c r="D33" s="79">
         <v>1000.0</v>
       </c>
-      <c r="E33" s="105"/>
-      <c r="F33" s="105"/>
+      <c r="E33" s="110"/>
+      <c r="F33" s="110"/>
       <c r="G33" s="23"/>
       <c r="H33" s="23"/>
       <c r="I33" s="23"/>
@@ -25725,8 +26108,8 @@
       <c r="D34" s="79">
         <v>998.7</v>
       </c>
-      <c r="E34" s="105"/>
-      <c r="F34" s="105"/>
+      <c r="E34" s="110"/>
+      <c r="F34" s="110"/>
       <c r="G34" s="23"/>
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
@@ -25746,8 +26129,8 @@
       <c r="D35" s="79">
         <v>998.3</v>
       </c>
-      <c r="E35" s="105"/>
-      <c r="F35" s="105"/>
+      <c r="E35" s="110"/>
+      <c r="F35" s="110"/>
       <c r="G35" s="23"/>
       <c r="H35" s="23"/>
       <c r="I35" s="23"/>
@@ -25756,7 +26139,7 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="28" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B36" s="79">
         <v>100.3</v>
@@ -25777,7 +26160,7 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="66" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B37" s="79">
         <v>99.4</v>
@@ -25798,7 +26181,7 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="66" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B38" s="79">
         <v>99.7</v>
@@ -25819,7 +26202,7 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="66" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B39" s="79">
         <v>99.8</v>
@@ -25891,43 +26274,43 @@
       <c r="K43" s="23"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="110"/>
-      <c r="B44" s="110"/>
-      <c r="C44" s="110"/>
-      <c r="D44" s="110"/>
-      <c r="E44" s="110"/>
-      <c r="F44" s="110"/>
-      <c r="G44" s="110"/>
-      <c r="H44" s="110"/>
-      <c r="I44" s="110"/>
-      <c r="J44" s="110"/>
-      <c r="K44" s="110"/>
+      <c r="A44" s="115"/>
+      <c r="B44" s="115"/>
+      <c r="C44" s="115"/>
+      <c r="D44" s="115"/>
+      <c r="E44" s="115"/>
+      <c r="F44" s="115"/>
+      <c r="G44" s="115"/>
+      <c r="H44" s="115"/>
+      <c r="I44" s="115"/>
+      <c r="J44" s="115"/>
+      <c r="K44" s="115"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="111"/>
-      <c r="B45" s="111"/>
-      <c r="C45" s="111"/>
-      <c r="D45" s="111"/>
-      <c r="E45" s="111"/>
-      <c r="F45" s="111"/>
-      <c r="G45" s="111"/>
-      <c r="H45" s="111"/>
-      <c r="I45" s="111"/>
-      <c r="J45" s="111"/>
-      <c r="K45" s="111"/>
+      <c r="A45" s="116"/>
+      <c r="B45" s="116"/>
+      <c r="C45" s="116"/>
+      <c r="D45" s="116"/>
+      <c r="E45" s="116"/>
+      <c r="F45" s="116"/>
+      <c r="G45" s="116"/>
+      <c r="H45" s="116"/>
+      <c r="I45" s="116"/>
+      <c r="J45" s="116"/>
+      <c r="K45" s="116"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="111"/>
-      <c r="B46" s="111"/>
-      <c r="C46" s="111"/>
-      <c r="D46" s="111"/>
-      <c r="E46" s="111"/>
-      <c r="F46" s="111"/>
-      <c r="G46" s="111"/>
-      <c r="H46" s="111"/>
-      <c r="I46" s="111"/>
-      <c r="J46" s="111"/>
-      <c r="K46" s="111"/>
+      <c r="A46" s="116"/>
+      <c r="B46" s="116"/>
+      <c r="C46" s="116"/>
+      <c r="D46" s="116"/>
+      <c r="E46" s="116"/>
+      <c r="F46" s="116"/>
+      <c r="G46" s="116"/>
+      <c r="H46" s="116"/>
+      <c r="I46" s="116"/>
+      <c r="J46" s="116"/>
+      <c r="K46" s="116"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="85" t="s">
@@ -26020,11 +26403,11 @@
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="107" t="s">
+      <c r="F52" s="112" t="s">
         <v>13</v>
       </c>
       <c r="H52" s="87" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -26036,7 +26419,7 @@
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="88" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="3"/>
@@ -26045,7 +26428,7 @@
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="88" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -26056,8 +26439,8 @@
         <v>18</v>
       </c>
       <c r="B54" s="14"/>
-      <c r="C54" s="108" t="s">
-        <v>209</v>
+      <c r="C54" s="113" t="s">
+        <v>213</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="17"/>
@@ -26077,7 +26460,7 @@
         <v>22</v>
       </c>
       <c r="B55" s="14"/>
-      <c r="C55" s="112">
+      <c r="C55" s="117">
         <v>245.0</v>
       </c>
       <c r="D55" s="2"/>
@@ -26095,19 +26478,19 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="B56" s="104" t="s">
-        <v>211</v>
+        <v>214</v>
+      </c>
+      <c r="B56" s="109" t="s">
+        <v>215</v>
       </c>
       <c r="C56" s="79" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D56" s="79" t="s">
-        <v>213</v>
-      </c>
-      <c r="E56" s="105"/>
-      <c r="F56" s="105"/>
+        <v>217</v>
+      </c>
+      <c r="E56" s="110"/>
+      <c r="F56" s="110"/>
       <c r="G56" s="23"/>
       <c r="H56" s="23"/>
       <c r="I56" s="23"/>
@@ -26118,7 +26501,7 @@
       <c r="A57" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="106">
+      <c r="B57" s="111">
         <v>4.9</v>
       </c>
       <c r="C57" s="79">
@@ -26127,8 +26510,8 @@
       <c r="D57" s="79">
         <v>49.9</v>
       </c>
-      <c r="E57" s="105"/>
-      <c r="F57" s="105"/>
+      <c r="E57" s="110"/>
+      <c r="F57" s="110"/>
       <c r="G57" s="23"/>
       <c r="H57" s="23"/>
       <c r="I57" s="23"/>
@@ -26148,8 +26531,8 @@
       <c r="D58" s="79">
         <v>49.7</v>
       </c>
-      <c r="E58" s="105"/>
-      <c r="F58" s="105"/>
+      <c r="E58" s="110"/>
+      <c r="F58" s="110"/>
       <c r="G58" s="23"/>
       <c r="H58" s="23"/>
       <c r="I58" s="23"/>
@@ -26158,7 +26541,7 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="28" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B59" s="79">
         <v>5.1</v>
@@ -26179,7 +26562,7 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="66" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B60" s="79">
         <v>5.2</v>
@@ -26200,7 +26583,7 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="66" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B61" s="79">
         <v>4.9</v>
@@ -26208,7 +26591,7 @@
       <c r="C61" s="79">
         <v>24.8</v>
       </c>
-      <c r="D61" s="106">
+      <c r="D61" s="111">
         <v>50.0</v>
       </c>
       <c r="E61" s="37"/>
@@ -26221,9 +26604,9 @@
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="66" t="s">
-        <v>217</v>
-      </c>
-      <c r="B62" s="106">
+        <v>221</v>
+      </c>
+      <c r="B62" s="111">
         <v>5.0</v>
       </c>
       <c r="C62" s="79">
@@ -26241,8 +26624,8 @@
       <c r="K62" s="23"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="113" t="s">
-        <v>228</v>
+      <c r="A63" s="118" t="s">
+        <v>232</v>
       </c>
       <c r="B63" s="29" t="str">
         <f>PROMEDIO</f>
@@ -26250,8 +26633,8 @@
       </c>
       <c r="C63" s="29"/>
       <c r="D63" s="29"/>
-      <c r="E63" s="113" t="s">
-        <v>229</v>
+      <c r="E63" s="118" t="s">
+        <v>233</v>
       </c>
       <c r="F63" s="23"/>
       <c r="G63" s="23"/>
@@ -26261,14 +26644,14 @@
       <c r="K63" s="23"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="113" t="s">
-        <v>230</v>
+      <c r="A64" s="118" t="s">
+        <v>234</v>
       </c>
       <c r="B64" s="29"/>
       <c r="C64" s="35"/>
       <c r="D64" s="35"/>
-      <c r="E64" s="113" t="s">
-        <v>231</v>
+      <c r="E64" s="118" t="s">
+        <v>235</v>
       </c>
       <c r="F64" s="23"/>
       <c r="G64" s="23"/>
@@ -26278,14 +26661,14 @@
       <c r="K64" s="23"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="113" t="s">
-        <v>232</v>
+      <c r="A65" s="118" t="s">
+        <v>236</v>
       </c>
       <c r="B65" s="29"/>
       <c r="C65" s="35"/>
       <c r="D65" s="35"/>
-      <c r="E65" s="113" t="s">
-        <v>233</v>
+      <c r="E65" s="118" t="s">
+        <v>237</v>
       </c>
       <c r="F65" s="23"/>
       <c r="G65" s="23"/>
@@ -26295,14 +26678,14 @@
       <c r="K65" s="23"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="113" t="s">
-        <v>234</v>
+      <c r="A66" s="118" t="s">
+        <v>238</v>
       </c>
       <c r="B66" s="35"/>
       <c r="C66" s="35"/>
       <c r="D66" s="35"/>
-      <c r="E66" s="113" t="s">
-        <v>231</v>
+      <c r="E66" s="118" t="s">
+        <v>235</v>
       </c>
       <c r="F66" s="23"/>
       <c r="G66" s="23"/>
@@ -26312,25 +26695,25 @@
       <c r="K66" s="23"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="114" t="s">
-        <v>235</v>
-      </c>
-      <c r="B67" s="114"/>
-      <c r="C67" s="114"/>
-      <c r="D67" s="114"/>
-      <c r="E67" s="114" t="s">
-        <v>229</v>
+      <c r="A67" s="119" t="s">
+        <v>239</v>
+      </c>
+      <c r="B67" s="119"/>
+      <c r="C67" s="119"/>
+      <c r="D67" s="119"/>
+      <c r="E67" s="119" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="114" t="s">
-        <v>236</v>
-      </c>
-      <c r="B68" s="114"/>
-      <c r="C68" s="114"/>
-      <c r="D68" s="114"/>
-      <c r="E68" s="114" t="s">
-        <v>233</v>
+      <c r="A68" s="119" t="s">
+        <v>240</v>
+      </c>
+      <c r="B68" s="119"/>
+      <c r="C68" s="119"/>
+      <c r="D68" s="119"/>
+      <c r="E68" s="119" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">

</xml_diff>